<commit_message>
update: Update trial organizations in users.xlsx
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -5,40 +5,57 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyuhyun/Documents/Users/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gyuhyun/Documents/streamlit_dashboard_new/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A0740B-F390-AF4A-A7DA-A2C345E53899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0B4B59-E45A-0C44-A755-BBDE3B48498C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{A7180B81-5BCA-C841-909A-097C3B0F75B3}"/>
   </bookViews>
   <sheets>
     <sheet name="date" sheetId="27" r:id="rId1"/>
-    <sheet name="bnp" sheetId="34" r:id="rId2"/>
-    <sheet name="bnp_invited" sheetId="35" r:id="rId3"/>
-    <sheet name="twinlions" sheetId="28" r:id="rId4"/>
-    <sheet name="twinlions_invited" sheetId="29" r:id="rId5"/>
-    <sheet name="blackstone" sheetId="30" r:id="rId6"/>
-    <sheet name="blackstone_invited" sheetId="31" r:id="rId7"/>
-    <sheet name="schonfeld" sheetId="32" r:id="rId8"/>
-    <sheet name="schonfeld_invited" sheetId="33" r:id="rId9"/>
-    <sheet name="carret" sheetId="1" r:id="rId10"/>
-    <sheet name="carret_invited" sheetId="2" r:id="rId11"/>
-    <sheet name="cgsi" sheetId="3" r:id="rId12"/>
-    <sheet name="cgsi_invited" sheetId="4" r:id="rId13"/>
-    <sheet name="macquarie" sheetId="5" r:id="rId14"/>
-    <sheet name="clsa" sheetId="7" r:id="rId15"/>
-    <sheet name="clsa_invited" sheetId="8" r:id="rId16"/>
-    <sheet name="anek" sheetId="9" r:id="rId17"/>
-    <sheet name="anek_invited" sheetId="10" r:id="rId18"/>
-    <sheet name="panvira" sheetId="11" r:id="rId19"/>
-    <sheet name="panvira_invited" sheetId="12" r:id="rId20"/>
-    <sheet name="rocksprings" sheetId="17" r:id="rId21"/>
-    <sheet name="rocksprings_invited" sheetId="18" r:id="rId22"/>
-    <sheet name="icici" sheetId="19" r:id="rId23"/>
-    <sheet name="j&amp;m_copper" sheetId="21" r:id="rId24"/>
-    <sheet name="redwood" sheetId="25" r:id="rId25"/>
-    <sheet name="redwood_invited" sheetId="26" r:id="rId26"/>
+    <sheet name="stefan" sheetId="53" r:id="rId2"/>
+    <sheet name="heinpark" sheetId="52" r:id="rId3"/>
+    <sheet name="cathay" sheetId="50" r:id="rId4"/>
+    <sheet name="cathay_invited" sheetId="51" r:id="rId5"/>
+    <sheet name="wedbush" sheetId="49" r:id="rId6"/>
+    <sheet name="janchor" sheetId="47" r:id="rId7"/>
+    <sheet name="causeway" sheetId="45" r:id="rId8"/>
+    <sheet name="causeway_invited" sheetId="46" r:id="rId9"/>
+    <sheet name="crescent" sheetId="43" r:id="rId10"/>
+    <sheet name="crescent_invited" sheetId="44" r:id="rId11"/>
+    <sheet name="thirdbridge" sheetId="41" r:id="rId12"/>
+    <sheet name="thirdbridge_invited" sheetId="42" r:id="rId13"/>
+    <sheet name="citigroup" sheetId="39" r:id="rId14"/>
+    <sheet name="coatue" sheetId="40" r:id="rId15"/>
+    <sheet name="trivest" sheetId="37" r:id="rId16"/>
+    <sheet name="trivest_invited" sheetId="38" r:id="rId17"/>
+    <sheet name="barclays" sheetId="36" r:id="rId18"/>
+    <sheet name="bnp" sheetId="34" r:id="rId19"/>
+    <sheet name="bnp_invited" sheetId="35" r:id="rId20"/>
+    <sheet name="twinlions" sheetId="28" r:id="rId21"/>
+    <sheet name="twinlions_invited" sheetId="29" r:id="rId22"/>
+    <sheet name="blackstone" sheetId="30" r:id="rId23"/>
+    <sheet name="blackstone_invited" sheetId="31" r:id="rId24"/>
+    <sheet name="schonfeld" sheetId="32" r:id="rId25"/>
+    <sheet name="schonfeld_invited" sheetId="33" r:id="rId26"/>
+    <sheet name="carret" sheetId="1" r:id="rId27"/>
+    <sheet name="carret_invited" sheetId="2" r:id="rId28"/>
+    <sheet name="cgsi" sheetId="3" r:id="rId29"/>
+    <sheet name="cgsi_invited" sheetId="4" r:id="rId30"/>
+    <sheet name="macquarie" sheetId="5" r:id="rId31"/>
+    <sheet name="clsa" sheetId="7" r:id="rId32"/>
+    <sheet name="clsa_invited" sheetId="8" r:id="rId33"/>
+    <sheet name="anek" sheetId="9" r:id="rId34"/>
+    <sheet name="anek_invited" sheetId="10" r:id="rId35"/>
+    <sheet name="panvira" sheetId="11" r:id="rId36"/>
+    <sheet name="panvira_invited" sheetId="12" r:id="rId37"/>
+    <sheet name="rocksprings" sheetId="17" r:id="rId38"/>
+    <sheet name="rocksprings_invited" sheetId="18" r:id="rId39"/>
+    <sheet name="icici" sheetId="19" r:id="rId40"/>
+    <sheet name="j&amp;m_copper" sheetId="21" r:id="rId41"/>
+    <sheet name="redwood" sheetId="25" r:id="rId42"/>
+    <sheet name="redwood_invited" sheetId="26" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="433">
   <si>
     <t>rachel.yin@carretprivate.com</t>
   </si>
@@ -992,13 +1009,400 @@
   </si>
   <si>
     <t>oliver.spensley@asia.bnpparibas.com</t>
+  </si>
+  <si>
+    <t>Barclays</t>
+  </si>
+  <si>
+    <t>Trivest Advisors</t>
+  </si>
+  <si>
+    <t>Third Bridge</t>
+  </si>
+  <si>
+    <t>Janchor Partners</t>
+  </si>
+  <si>
+    <t>Cathay Holdings</t>
+  </si>
+  <si>
+    <t>Stefan Chang</t>
+  </si>
+  <si>
+    <t>hariom_tatsat@mfe.berkeley.edu</t>
+  </si>
+  <si>
+    <t>Harion Tatsat</t>
+  </si>
+  <si>
+    <t>Paying</t>
+  </si>
+  <si>
+    <t>yangxue.wu@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Yangxue</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>allen.lee@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>allen.lee</t>
+  </si>
+  <si>
+    <t>jack.wei@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>jack.wei</t>
+  </si>
+  <si>
+    <t>lan.xue@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>lan.xue</t>
+  </si>
+  <si>
+    <t>elsie.cheng@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Elsie Haiwen Cheng</t>
+  </si>
+  <si>
+    <t>blocked</t>
+  </si>
+  <si>
+    <t>helen.lou@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Helen LOU</t>
+  </si>
+  <si>
+    <t>shuo.yang@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Shuo Yang</t>
+  </si>
+  <si>
+    <t>shida.zhang@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>shida.zhang</t>
+  </si>
+  <si>
+    <t>steven.chen@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>steven.chen</t>
+  </si>
+  <si>
+    <t>ian.wang@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>ian.wang</t>
+  </si>
+  <si>
+    <t>lu.sun@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>lu.sun</t>
+  </si>
+  <si>
+    <t>jintian.mei@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>simon mei</t>
+  </si>
+  <si>
+    <t>sunkey.wang@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Sunkey Wang</t>
+  </si>
+  <si>
+    <t>evan.bi@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Zhongyuan BI</t>
+  </si>
+  <si>
+    <t>erica.xie@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Erica Xie</t>
+  </si>
+  <si>
+    <t>nan.jiang@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>jiang nan</t>
+  </si>
+  <si>
+    <t>qiqi.wang@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Qiqi Wang</t>
+  </si>
+  <si>
+    <t>jason.he@trivest-advisors.com</t>
+  </si>
+  <si>
+    <t>Tirvest Advisors</t>
+  </si>
+  <si>
+    <t>Citigroup</t>
+  </si>
+  <si>
+    <t>josh.yang@citi.com</t>
+  </si>
+  <si>
+    <t>Josh YAng</t>
+  </si>
+  <si>
+    <t>peter.sc.lee@citi.com</t>
+  </si>
+  <si>
+    <t>Peter Lee</t>
+  </si>
+  <si>
+    <t>Coatue Management</t>
+  </si>
+  <si>
+    <t>dzhengzhi@coatue.com</t>
+  </si>
+  <si>
+    <t>Donald Zheng</t>
+  </si>
+  <si>
+    <t>cpackard@coatue.com</t>
+  </si>
+  <si>
+    <t>Chase Packard</t>
+  </si>
+  <si>
+    <t>simon.zhai@thirdbridge.com</t>
+  </si>
+  <si>
+    <t>Zhai Simon</t>
+  </si>
+  <si>
+    <t>tony.yin@thirdbridge.com</t>
+  </si>
+  <si>
+    <t>Yin Tony</t>
+  </si>
+  <si>
+    <t>claudio.xia-api-user@thirdbridge.com</t>
+  </si>
+  <si>
+    <t>Claudio Xia API User</t>
+  </si>
+  <si>
+    <t>claudio.xia@thirdbridge.com</t>
+  </si>
+  <si>
+    <t>Claudio Xia</t>
+  </si>
+  <si>
+    <t>destin.cao@thirdbridge.com</t>
+  </si>
+  <si>
+    <t>Crescent Rock Capital Management</t>
+  </si>
+  <si>
+    <t>john@crescentrockcapital.com</t>
+  </si>
+  <si>
+    <t>John Rolfe</t>
+  </si>
+  <si>
+    <t>scott@crescentrockcapital.com</t>
+  </si>
+  <si>
+    <t>Scott Mosberg</t>
+  </si>
+  <si>
+    <t>michael@crescentrockcapital.com</t>
+  </si>
+  <si>
+    <t>Michael Marone</t>
+  </si>
+  <si>
+    <t>Crescent Rock Capital Managmenet</t>
+  </si>
+  <si>
+    <t>boris@crescentrockcapital.com</t>
+  </si>
+  <si>
+    <t>chris@crescentrockcapital.com</t>
+  </si>
+  <si>
+    <t>Causeway Capital</t>
+  </si>
+  <si>
+    <t>akc@causewaycap.com</t>
+  </si>
+  <si>
+    <t>Ajay Kc</t>
+  </si>
+  <si>
+    <t>ppetersen@causewaycap.com</t>
+  </si>
+  <si>
+    <t>Pete Peterson</t>
+  </si>
+  <si>
+    <t>nchang@causewaycap.com</t>
+  </si>
+  <si>
+    <t>Nathan Chang</t>
+  </si>
+  <si>
+    <t>ppetersen-api-user@causewaycap.com</t>
+  </si>
+  <si>
+    <t>Pete Peterson API User</t>
+  </si>
+  <si>
+    <t>ngibson@causewaycap.com</t>
+  </si>
+  <si>
+    <t>swilson@causewaycap.com</t>
+  </si>
+  <si>
+    <t>admin@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>Admin Janchor</t>
+  </si>
+  <si>
+    <t>qiang.wang@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>qiang wang</t>
+  </si>
+  <si>
+    <t>shelley.wang@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>Shelley Wang</t>
+  </si>
+  <si>
+    <t>kelly.chan@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>Kelly Chan</t>
+  </si>
+  <si>
+    <t>tian.ren@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>TIAN REN</t>
+  </si>
+  <si>
+    <t>john.ho@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>John Ho</t>
+  </si>
+  <si>
+    <t>janchor_partners@api_user.com</t>
+  </si>
+  <si>
+    <t>Janchor Partners API User</t>
+  </si>
+  <si>
+    <t>rebecca.lo@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>Rebecca Lo</t>
+  </si>
+  <si>
+    <t>flora.liao@janchorpartners.com</t>
+  </si>
+  <si>
+    <t>Flora Liao</t>
+  </si>
+  <si>
+    <t>Wedbush Securities</t>
+  </si>
+  <si>
+    <t>ariel.katz@wedbush.com</t>
+  </si>
+  <si>
+    <t>Ariel Katz</t>
+  </si>
+  <si>
+    <t>jeanlouis.lee@wedbush.com</t>
+  </si>
+  <si>
+    <t>Jean Louis Lee</t>
+  </si>
+  <si>
+    <t>jinjoo.hong@wedbush.com</t>
+  </si>
+  <si>
+    <t>Jinjoo Hong</t>
+  </si>
+  <si>
+    <t>monicakuo@cathayholdings.com.tw</t>
+  </si>
+  <si>
+    <t>Monica Kuo</t>
+  </si>
+  <si>
+    <t>jeff.yen@cathayholdings.com.tw</t>
+  </si>
+  <si>
+    <t>Jeff Yen</t>
+  </si>
+  <si>
+    <t>ericchao@cathayholdings.com.tw</t>
+  </si>
+  <si>
+    <t>Eric Chao</t>
+  </si>
+  <si>
+    <t>cathay_holdings@api_user.com</t>
+  </si>
+  <si>
+    <t>Cathay Holdings API User</t>
+  </si>
+  <si>
+    <t>annie.lee@cathaysec.com.tw</t>
+  </si>
+  <si>
+    <t>marschuang@cathaysec.com.tw</t>
+  </si>
+  <si>
+    <t>ella.hou@cathaysec.com.tw</t>
+  </si>
+  <si>
+    <t>Hein Park Capital</t>
+  </si>
+  <si>
+    <t>jwang@heinpark.com</t>
+  </si>
+  <si>
+    <t>Justin Wang</t>
+  </si>
+  <si>
+    <t>aha@heinpark.com</t>
+  </si>
+  <si>
+    <t>Arnold Ha</t>
+  </si>
+  <si>
+    <t>stefanchang@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1098,6 +1502,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1124,7 +1534,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1171,6 +1581,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1508,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FE63AB-45E9-904A-AE86-5E5A4A005740}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,37 +2128,147 @@
       <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" s="8">
+        <v>45852</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="8">
+        <v>45469</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17" s="8">
+        <v>45866</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="B18" s="8">
+        <v>45867</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" s="8">
+        <v>45804</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B20" s="8">
+        <v>45869</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B21" s="15">
+        <v>45817</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" s="8">
+        <v>45810</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="B23" s="8">
+        <v>45866</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B24" s="8">
+        <v>45870</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="8:8" ht="19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="B25" s="8">
+        <v>45869</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>285</v>
+      </c>
       <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B26" s="8">
+        <v>45870</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>285</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1753,6 +2276,1788 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64897F78-4E95-7942-88CC-0179A26F9ACE}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C3" t="s">
+        <v>377</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B34A4B8-C631-8143-BB00-E2815E6BA075}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8CB2E2-C0FA-344E-BC94-83D141B2C520}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A72524-0CDA-6F47-9FB1-7368D991B0D8}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116B5286-D570-DF4A-938C-477352B816B1}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC34782-0D41-BE4D-A580-C63699011A6B}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F4E792-0543-0C48-9A24-170CAE99EB74}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C16" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C17" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41985BEC-907B-8A47-8B3C-55DEDB7AD105}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA91D01-0E02-504C-A8E0-E4A8C5AE43F9}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70DABA4-D73A-9C4A-BD45-3FFC84BF05F3}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="D10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811BF58-2CD2-2247-9792-9B3FF8245338}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03170CD5-5125-934F-A115-1D17DE7153AF}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E12DC6-3338-F245-A865-681D2CEB9666}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC15DED-FF42-D74E-B42B-C5DC15A732DE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CC2D23-B13F-4447-8534-C9D95D831AFB}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAB494C-3F81-EC48-960A-399A209E4687}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{773EF47C-ABDA-2B4A-B5AE-B91E45AC94FC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDC1DA0-7B88-1E42-A9E3-3A54D29AD15F}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CB7590-605D-8449-B2FD-96C21A5A1416}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{954D22C4-69EE-EE49-A97B-EE58C459D581}">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -2023,7 +4328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B2AB4A-3ABC-9244-B8C5-FE46542EE78D}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -2082,7 +4387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA517709-6AD5-EB47-A072-569CF8321F17}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2393,7 +4698,77 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD397864-7418-E640-9B30-E7E2D25019B2}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16D7783-4037-F648-9880-98E87D4D1115}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -2466,7 +4841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2577BC-8E86-8442-B0D0-E8149C958E66}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -2769,7 +5144,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B76C5C3-FCF7-7643-BB3D-9A0D6591C2D8}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2991,7 +5366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBF9DA1-0027-4646-984D-477CA814F6AA}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -3204,7 +5579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD7BE0E-3A9C-3C4B-AD88-E42C390A0042}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -3268,7 +5643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AB057C-AAB7-304B-8B03-D91946C03157}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -3338,7 +5713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BD8450-3D6A-2844-B51B-4BB55AADF2F6}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3399,174 +5774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70DABA4-D73A-9C4A-BD45-3FFC84BF05F3}">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C6" t="s">
-        <v>287</v>
-      </c>
-      <c r="D6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="D9" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="D10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCF1C8E-491F-D84F-B8C6-D75AE41E676E}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -3631,7 +5839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171458C0-70BA-BB43-97B3-819816159727}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -3776,7 +5984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F8C68A-B9BA-9743-BE06-2841AAAA9C55}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3819,7 +6027,115 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18408018-B24C-C848-8FCA-36330368A4AB}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5849B3EF-4806-7646-80B0-1F8B3F584CC7}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -3900,7 +6216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D26009C-03B2-E14D-A4A0-339B3D7C115B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3954,7 +6270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8AD43AC-2D64-9042-9D64-4C344B77958F}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4000,7 +6316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0C1005-93B6-B545-96A6-84A08D6CABE3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4035,12 +6351,166 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03170CD5-5125-934F-A115-1D17DE7153AF}">
-  <dimension ref="A1:H3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65F1EF6-9FD5-6B47-B91A-DE47510CCF6E}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95775B31-55C2-064A-B28D-4A4B88D339B5}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="B2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8924A50-A599-0044-9121-3B47011A8463}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4050,49 +6520,191 @@
         <v>30</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>302</v>
+        <v>391</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>287</v>
+        <v>392</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+        <v>307</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>303</v>
+        <v>393</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>287</v>
+        <v>394</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C10" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E12DC6-3338-F245-A865-681D2CEB9666}">
-  <dimension ref="A1:I3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B73E56-8500-EF42-AE4A-88081B5A82FF}">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -4119,17 +6731,15 @@
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>234</v>
+        <v>381</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>192</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -4137,507 +6747,48 @@
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>236</v>
+        <v>383</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>192</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="C3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC15DED-FF42-D74E-B42B-C5DC15A732DE}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CC2D23-B13F-4447-8534-C9D95D831AFB}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>243</v>
+        <v>385</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>192</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="C4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAB494C-3F81-EC48-960A-399A209E4687}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{773EF47C-ABDA-2B4A-B5AE-B91E45AC94FC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADDC1DA0-7B88-1E42-A9E3-3A54D29AD15F}">
-  <dimension ref="A1:H18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>254</v>
+        <v>387</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+        <v>388</v>
+      </c>
+      <c r="C5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="I5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4645,11 +6796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CB7590-605D-8449-B2FD-96C21A5A1416}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9671278A-72E9-2840-AE2D-9A3E20D7002E}">
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4667,53 +6818,53 @@
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>231</v>
+        <v>389</v>
+      </c>
+      <c r="B2" t="s">
+        <v>380</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>231</v>
+        <v>390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>380</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="D5" s="1"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>